<commit_message>
1. Created a report template (Excel file) in REFramework's Output folder. 2. Added the the report's file path in the Config file. 3. Added logic to the Set Transaction Status workflow so that each transaction's status is updated in an Excel file.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>UiDemo_app\UiDemo.exe</t>
+  </si>
+  <si>
+    <t>StatusFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\Status.xlsx</t>
   </si>
 </sst>
 </file>
@@ -550,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -646,7 +652,14 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2806,7 +2819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>